<commit_message>
key milestones and key dependences
</commit_message>
<xml_diff>
--- a/TERM3/T3B1-ICTPMG613-Manage_ICT_project_plan/2-ICTPMG613-Assessment_Task 2/ICTPMG613_AssessmentTask_Manuel_S_Perez_E-Pert_Chart.xlsx
+++ b/TERM3/T3B1-ICTPMG613-Manage_ICT_project_plan/2-ICTPMG613-Assessment_Task 2/ICTPMG613_AssessmentTask_Manuel_S_Perez_E-Pert_Chart.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\Assessments\TERM3\T3B1-ICTPMG613-Manage_ICT_project_plan\2-ICTPMG613-Assessment_Task 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5E7209-5FC5-4607-8B25-CB2E616CBD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975F674F-E303-4B99-81AC-F85AA9C1F7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E7573F3-6188-4FA9-9041-50436B486355}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="2" xr2:uid="{2E7573F3-6188-4FA9-9041-50436B486355}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart" sheetId="1" r:id="rId1"/>
+    <sheet name="k-Milestones" sheetId="2" r:id="rId2"/>
+    <sheet name="k-Dependences" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="186">
   <si>
     <t>Activity</t>
   </si>
@@ -510,17 +512,102 @@
   </si>
   <si>
     <t>Unintuitive design, lack of client commitment</t>
+  </si>
+  <si>
+    <t>Project Charters Approved</t>
+  </si>
+  <si>
+    <t>Kickoff Meetings Conducted</t>
+  </si>
+  <si>
+    <t>Project Plans Approved</t>
+  </si>
+  <si>
+    <t>Cloud Provider Contract Signed</t>
+  </si>
+  <si>
+    <t>Cloud Infrastructure Configured</t>
+  </si>
+  <si>
+    <t>Databases Successfully Migrated</t>
+  </si>
+  <si>
+    <t>Core Applications Deployed to Cloud</t>
+  </si>
+  <si>
+    <t>Devices Distributed and Configured</t>
+  </si>
+  <si>
+    <t>Training Completed</t>
+  </si>
+  <si>
+    <t>First Sprint Completed &amp; Reviewed</t>
+  </si>
+  <si>
+    <t>Website Deployed to Production</t>
+  </si>
+  <si>
+    <t>Formal Project Closure</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Milestone</t>
+  </si>
+  <si>
+    <t>Depedency</t>
+  </si>
+  <si>
+    <t>Gain Formal Acceptance of Project Charter</t>
+  </si>
+  <si>
+    <t>Gain Formal Acceptance of Scope Statement</t>
+  </si>
+  <si>
+    <t>Gain Formal Acceptance of Project Plans</t>
+  </si>
+  <si>
+    <t>Formal budget obtaining</t>
+  </si>
+  <si>
+    <t>Select Cloud Provider and Sign Contract</t>
+  </si>
+  <si>
+    <t>Migrate Databases to a Cloud platform</t>
+  </si>
+  <si>
+    <t>Develop and Deploy Core Applications to Cloud platform</t>
+  </si>
+  <si>
+    <t>Perform System-Wide Testing</t>
+  </si>
+  <si>
+    <t>Select work devices Provider and Sign Contract</t>
+  </si>
+  <si>
+    <t>Configure Work Devices</t>
+  </si>
+  <si>
+    <t>Gain Formal Acceptance of website functionalities</t>
+  </si>
+  <si>
+    <t>Conduct Final Testing: IT infrastructure and website, and remote connection</t>
+  </si>
+  <si>
+    <t>Due Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,###&quot; days&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot; days&quot;"/>
+    <numFmt numFmtId="166" formatCode="ddd\ dd/mmm/yy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,6 +630,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -558,7 +663,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -644,12 +749,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -696,9 +817,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{BB0E93A7-55F0-4420-8B0A-8DA068096FC5}"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1033,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCCED96-865F-42B1-814A-F0DD7A1F90A0}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1042,7 +1181,7 @@
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="9.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" style="1" customWidth="1"/>
     <col min="8" max="8" width="28.21875" style="1" customWidth="1"/>
@@ -3011,4 +3150,312 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081C22EC-4620-4117-A76D-1E4837839DB1}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="19">
+        <v>45874</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="17">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="20">
+        <v>45877</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="17">
+        <f t="shared" ref="A4:A13" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="20">
+        <v>45877</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="20">
+        <v>45881</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="20">
+        <v>45889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="20">
+        <v>45889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="20">
+        <v>45897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="20">
+        <v>45901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="17">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="20">
+        <v>45917</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="20">
+        <v>45898</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="20">
+        <v>45901</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="20">
+        <v>45929</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A6C9D0-B316-4A49-8090-E1E0626B3E1F}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="17">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="17">
+        <f t="shared" ref="A4:A13" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="17">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
edning... applying style 613
</commit_message>
<xml_diff>
--- a/TERM3/T3B1-ICTPMG613-Manage_ICT_project_plan/2-ICTPMG613-Assessment_Task 2/ICTPMG613_AssessmentTask_Manuel_S_Perez_E-Pert_Chart.xlsx
+++ b/TERM3/T3B1-ICTPMG613-Manage_ICT_project_plan/2-ICTPMG613-Assessment_Task 2/ICTPMG613_AssessmentTask_Manuel_S_Perez_E-Pert_Chart.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\Assessments\TERM3\T3B1-ICTPMG613-Manage_ICT_project_plan\2-ICTPMG613-Assessment_Task 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE80812E-588D-4469-B5BB-314D80DD20CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26C845B-7D6B-4B85-97FB-306127DB811A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E7573F3-6188-4FA9-9041-50436B486355}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart" sheetId="1" r:id="rId1"/>
     <sheet name="k-Milestones" sheetId="2" r:id="rId2"/>
-    <sheet name="k-Dependences" sheetId="3" r:id="rId3"/>
-    <sheet name="Change-control" sheetId="4" r:id="rId4"/>
-    <sheet name="Comms-control" sheetId="5" r:id="rId5"/>
-    <sheet name="Comms-directory" sheetId="6" r:id="rId6"/>
+    <sheet name="QA-baseline" sheetId="7" r:id="rId3"/>
+    <sheet name="k-Dependences" sheetId="3" r:id="rId4"/>
+    <sheet name="Change-control" sheetId="4" r:id="rId5"/>
+    <sheet name="Comms-control" sheetId="5" r:id="rId6"/>
+    <sheet name="Comms-directory" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="316">
   <si>
     <t>Activity</t>
   </si>
@@ -947,6 +948,48 @@
   </si>
   <si>
     <t>susan.mor@boutiquebuild.com.au</t>
+  </si>
+  <si>
+    <t>New Cloud-Based IT Infrastructure with Scalable, Fault-Tolerant Core Applications</t>
+  </si>
+  <si>
+    <t>Infrastructure fully configured, operational, and fault-tolerant; core applications meet performance, security, and functionality standards</t>
+  </si>
+  <si>
+    <t>Zero critical failures; maximum of 2 minor configuration or performance issues</t>
+  </si>
+  <si>
+    <t>Modern, High-Quality, Engaging, and Stylish Website</t>
+  </si>
+  <si>
+    <t>Website meets usability, design, and performance standards; fully functional with no critical bugs; load times optimized</t>
+  </si>
+  <si>
+    <t>Zero critical defects; maximum of 5 minor defects; page load time ≤ 3 seconds</t>
+  </si>
+  <si>
+    <t>Remote Access Tools and Fully Distributed Work Devices</t>
+  </si>
+  <si>
+    <t>All devices correctly configured and connected; remote access tools fully functional and secure</t>
+  </si>
+  <si>
+    <t>Zero critical connectivity failures; maximum 5% minor configuration issues</t>
+  </si>
+  <si>
+    <t>Comprehensive Documentation and Training</t>
+  </si>
+  <si>
+    <t>All documentation complete, accurate, and understandable; staff training delivered and effective</t>
+  </si>
+  <si>
+    <t>Minimum 90% staff satisfaction; maximum 5% minor documentation errors</t>
+  </si>
+  <si>
+    <t>QA Indicator</t>
+  </si>
+  <si>
+    <t>Acceptable Level</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1135,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1186,13 +1229,19 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -1535,8 +1584,8 @@
   </sheetPr>
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3519,8 +3568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081C22EC-4620-4117-A76D-1E4837839DB1}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3731,11 +3780,86 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52962F3B-7E13-4F4A-95DB-0576158409CF}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>305</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A6C9D0-B316-4A49-8090-E1E0626B3E1F}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="A1:XFD1048576"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3865,12 +3989,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4A8877-E8DA-4C66-94BC-D151587F6D20}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D16" sqref="A11:D19"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3883,12 +4007,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -4001,12 +4125,12 @@
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="34" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
@@ -4130,7 +4254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0362EF11-4C07-4F65-A6EC-3FC0EC3607B0}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -4293,11 +4417,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{076153BA-5795-42F2-906B-9931FC8D5804}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -4470,7 +4594,7 @@
       <c r="B10" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="33" t="s">
         <v>301</v>
       </c>
       <c r="D10" s="5" t="s">

</xml_diff>